<commit_message>
Update time domain paper results with more-accurate numbers
</commit_message>
<xml_diff>
--- a/TimeDomainPaper/SiVH3/results/Si_4x4x4_0th_20230823_new_lattice_constant.xlsx
+++ b/TimeDomainPaper/SiVH3/results/Si_4x4x4_0th_20230823_new_lattice_constant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1e31cf061855cba/MyStuff/Research/Vanderbilt/CrossSectionCalculations/SiVH3/GaNPaper/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1e31cf061855cba/MyStuff/Research/Vanderbilt/CrossSectionCalculations/TimeDomainPaper/SiVH3/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="588" documentId="8_{8FCC5D58-F92F-4816-9671-755DACE29FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A61BA3AC-9642-4486-9616-9ABAB1E64227}"/>
+  <xr:revisionPtr revIDLastSave="593" documentId="8_{8FCC5D58-F92F-4816-9671-755DACE29FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{441FB256-4B29-4242-B069-1ED8707EA256}"/>
   <bookViews>
     <workbookView xWindow="34450" yWindow="5380" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{CE35B33A-17EB-4004-BCB0-DD5C2147CA48}"/>
   </bookViews>
@@ -240,10 +240,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2843,15 +2839,15 @@
       </c>
       <c r="U3" s="3">
         <f>'Laura Raw Data Pos'!F2*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P3</f>
-        <v>5.8999892725645007E-21</v>
+        <v>6.1049417080791902E-21</v>
       </c>
       <c r="V3" s="3">
         <f t="shared" ref="V3:V32" si="0">U3/T3</f>
-        <v>2.4309591860888818E-4</v>
+        <v>2.5154052728203517E-4</v>
       </c>
       <c r="W3" s="3">
         <f>SUMPRODUCT(V3:V66, T3:T66) / SUM(T3:T66)</f>
-        <v>1.2653644202442079E-3</v>
+        <v>3.7092781264699746E-3</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -2920,11 +2916,11 @@
       </c>
       <c r="U4" s="3">
         <f>'Laura Raw Data Pos'!F3*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P4</f>
-        <v>1.8775976326239294E-21</v>
+        <v>3.5235402873147855E-21</v>
       </c>
       <c r="V4" s="3">
         <f t="shared" si="0"/>
-        <v>1.6106640123110782E-4</v>
+        <v>3.0226068877041852E-4</v>
       </c>
       <c r="W4" s="3"/>
     </row>
@@ -2994,11 +2990,11 @@
       </c>
       <c r="U5" s="3">
         <f>'Laura Raw Data Pos'!F4*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P5</f>
-        <v>1.7629345085802314E-21</v>
+        <v>1.921272642322668E-21</v>
       </c>
       <c r="V5" s="3">
         <f t="shared" si="0"/>
-        <v>4.2810605185378331E-5</v>
+        <v>4.6655643839080879E-5</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -3067,11 +3063,11 @@
       </c>
       <c r="U6" s="3">
         <f>'Laura Raw Data Pos'!F5*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P6</f>
-        <v>2.6813589412635368E-21</v>
+        <v>2.9202337260454646E-21</v>
       </c>
       <c r="V6" s="3">
         <f t="shared" si="0"/>
-        <v>2.0308192642552573E-4</v>
+        <v>2.211739284777153E-4</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -3140,11 +3136,11 @@
       </c>
       <c r="U7" s="3">
         <f>'Laura Raw Data Pos'!F6*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P7</f>
-        <v>1.4339836989747264E-19</v>
+        <v>1.4791179737441412E-19</v>
       </c>
       <c r="V7" s="3">
         <f t="shared" si="0"/>
-        <v>3.9812590788882662E-2</v>
+        <v>4.1065682029203222E-2</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -3213,11 +3209,11 @@
       </c>
       <c r="U8" s="3">
         <f>'Laura Raw Data Pos'!F7*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P8</f>
-        <v>6.9511182913788217E-21</v>
+        <v>1.1107658588786844E-19</v>
       </c>
       <c r="V8" s="3">
         <f t="shared" si="0"/>
-        <v>1.1246610418830832E-4</v>
+        <v>1.7971713841843727E-3</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -3286,11 +3282,11 @@
       </c>
       <c r="U9" s="3">
         <f>'Laura Raw Data Pos'!F8*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P9</f>
-        <v>3.4107394064063889E-21</v>
+        <v>4.4190558967624266E-20</v>
       </c>
       <c r="V9" s="3">
         <f t="shared" si="0"/>
-        <v>54.301995227053595</v>
+        <v>703.55287701943155</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -3359,11 +3355,11 @@
       </c>
       <c r="U10" s="3">
         <f>'Laura Raw Data Pos'!F9*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P10</f>
-        <v>4.7263481643163129E-20</v>
+        <v>4.7690104075583482E-20</v>
       </c>
       <c r="V10" s="3">
         <f t="shared" si="0"/>
-        <v>442.47030161384532</v>
+        <v>446.46424682874618</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -3432,11 +3428,11 @@
       </c>
       <c r="U11" s="3">
         <f>'Laura Raw Data Pos'!F10*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P11</f>
-        <v>1.0669891477295195E-21</v>
+        <v>1.0957632053211248E-21</v>
       </c>
       <c r="V11" s="3">
         <f t="shared" si="0"/>
-        <v>3.6978842049076595E-5</v>
+        <v>3.7976069933779257E-5</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -3505,11 +3501,11 @@
       </c>
       <c r="U12" s="3">
         <f>'Laura Raw Data Pos'!F11*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P12</f>
-        <v>9.1310496801733567E-21</v>
+        <v>9.2428614085155025E-21</v>
       </c>
       <c r="V12" s="3">
         <f t="shared" si="0"/>
-        <v>8.5671642173421204E-3</v>
+        <v>8.672071043138059E-3</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -3578,11 +3574,11 @@
       </c>
       <c r="U13" s="3">
         <f>'Laura Raw Data Pos'!F12*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P13</f>
-        <v>6.3027604893330412E-21</v>
+        <v>6.4126588717715257E-21</v>
       </c>
       <c r="V13" s="3">
         <f t="shared" si="0"/>
-        <v>2.3116139466766314E-2</v>
+        <v>2.3519205129807059E-2</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -3651,11 +3647,11 @@
       </c>
       <c r="U14" s="3">
         <f>'Laura Raw Data Pos'!F13*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P14</f>
-        <v>3.0071840990939899E-21</v>
+        <v>5.2716345958709735E-21</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="0"/>
-        <v>6.4860598591029689E-4</v>
+        <v>1.1370151084012015E-3</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -3724,11 +3720,11 @@
       </c>
       <c r="U15" s="3">
         <f>'Laura Raw Data Pos'!F14*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P15</f>
-        <v>5.0596035012244405E-22</v>
+        <v>5.440632335583149E-22</v>
       </c>
       <c r="V15" s="3">
         <f t="shared" si="0"/>
-        <v>2.4682346111033929E-2</v>
+        <v>2.6541125275379412E-2</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -3797,11 +3793,11 @@
       </c>
       <c r="U16" s="3">
         <f>'Laura Raw Data Pos'!F15*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P16</f>
-        <v>1.2700367363616497E-22</v>
+        <v>1.313862667977622E-22</v>
       </c>
       <c r="V16" s="3">
         <f t="shared" si="0"/>
-        <v>4.3802707237545985E-5</v>
+        <v>4.5314233949353244E-5</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -3870,11 +3866,11 @@
       </c>
       <c r="U17" s="3">
         <f>'Laura Raw Data Pos'!F16*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P17</f>
-        <v>1.5780280945534419E-22</v>
+        <v>6.4100349345861923E-22</v>
       </c>
       <c r="V17" s="3">
         <f t="shared" si="0"/>
-        <v>2.6464234773110955E-5</v>
+        <v>1.0749914402552924E-4</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -3943,11 +3939,11 @@
       </c>
       <c r="U18" s="3">
         <f>'Laura Raw Data Pos'!F17*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P18</f>
-        <v>8.8575056089994172E-21</v>
+        <v>8.9307755684074292E-21</v>
       </c>
       <c r="V18" s="3">
         <f t="shared" si="0"/>
-        <v>7.0758930985128929E-3</v>
+        <v>7.1344254238638032E-3</v>
       </c>
     </row>
     <row r="19" spans="1:22">
@@ -4016,11 +4012,11 @@
       </c>
       <c r="U19" s="3">
         <f>'Laura Raw Data Pos'!F18*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P19</f>
-        <v>3.0309252018340611E-22</v>
+        <v>3.9311075429677628E-22</v>
       </c>
       <c r="V19" s="3">
         <f t="shared" si="0"/>
-        <v>7.9545948319004519E-3</v>
+        <v>1.0317103083247998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -4089,11 +4085,11 @@
       </c>
       <c r="U20" s="3">
         <f>'Laura Raw Data Pos'!F19*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P20</f>
-        <v>3.7834423185064527E-22</v>
+        <v>4.2989076299449149E-21</v>
       </c>
       <c r="V20" s="3">
         <f t="shared" si="0"/>
-        <v>1.0781295269441076E-3</v>
+        <v>1.2250164953693667E-2</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -4162,11 +4158,11 @@
       </c>
       <c r="U21" s="3">
         <f>'Laura Raw Data Pos'!F20*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P21</f>
-        <v>3.0454684097430058E-22</v>
+        <v>9.3523770933135325E-21</v>
       </c>
       <c r="V21" s="3">
         <f t="shared" si="0"/>
-        <v>9.1278170516621349E-4</v>
+        <v>2.8030757709657333E-2</v>
       </c>
     </row>
     <row r="22" spans="1:22">
@@ -4235,11 +4231,11 @@
       </c>
       <c r="U22" s="3">
         <f>'Laura Raw Data Pos'!F21*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P22</f>
-        <v>1.69389368086134E-22</v>
+        <v>2.1820153718781444E-22</v>
       </c>
       <c r="V22" s="3">
         <f t="shared" si="0"/>
-        <v>1.4746849741667823E-4</v>
+        <v>1.8996382822996356E-4</v>
       </c>
     </row>
     <row r="23" spans="1:22">
@@ -4308,11 +4304,11 @@
       </c>
       <c r="U23" s="3">
         <f>'Laura Raw Data Pos'!F22*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P23</f>
-        <v>1.551619687673949E-22</v>
+        <v>1.8211745519366722E-22</v>
       </c>
       <c r="V23" s="3">
         <f t="shared" si="0"/>
-        <v>2.5279522768540633E-4</v>
+        <v>2.9671203528093033E-4</v>
       </c>
     </row>
     <row r="24" spans="1:22">
@@ -4381,11 +4377,11 @@
       </c>
       <c r="U24" s="3">
         <f>'Laura Raw Data Pos'!F23*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P24</f>
-        <v>2.9035105140250827E-21</v>
+        <v>2.9239401992174318E-21</v>
       </c>
       <c r="V24" s="3">
         <f t="shared" si="0"/>
-        <v>6.4142160115273567E-3</v>
+        <v>6.4593477281986939E-3</v>
       </c>
     </row>
     <row r="25" spans="1:22">
@@ -4454,11 +4450,11 @@
       </c>
       <c r="U25" s="3">
         <f>'Laura Raw Data Pos'!F24*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P25</f>
-        <v>1.5147164775645094E-22</v>
+        <v>2.1987330053500666E-22</v>
       </c>
       <c r="V25" s="3">
         <f t="shared" si="0"/>
-        <v>7.3428939777322967E-5</v>
+        <v>1.0658802213326187E-4</v>
       </c>
     </row>
     <row r="26" spans="1:22">
@@ -4527,11 +4523,11 @@
       </c>
       <c r="U26" s="3">
         <f>'Laura Raw Data Pos'!F25*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P26</f>
-        <v>2.1036719726680557E-22</v>
+        <v>2.2049338466428933E-22</v>
       </c>
       <c r="V26" s="3">
         <f t="shared" si="0"/>
-        <v>1.5720886683557542E-4</v>
+        <v>1.6477623697125343E-4</v>
       </c>
     </row>
     <row r="27" spans="1:22">
@@ -4600,11 +4596,11 @@
       </c>
       <c r="U27" s="3">
         <f>'Laura Raw Data Pos'!F26*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P27</f>
-        <v>8.1296097506936999E-22</v>
+        <v>8.9235149554342255E-20</v>
       </c>
       <c r="V27" s="3">
         <f t="shared" si="0"/>
-        <v>1.1914735289344852E-3</v>
+        <v>0.13078280729949715</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -4673,11 +4669,11 @@
       </c>
       <c r="U28" s="3">
         <f>'Laura Raw Data Pos'!F27*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P28</f>
-        <v>1.4909264476926304E-22</v>
+        <v>1.7063729528513625E-22</v>
       </c>
       <c r="V28" s="3">
         <f t="shared" si="0"/>
-        <v>1.1271768538023621E-4</v>
+        <v>1.2900596802646364E-4</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -4746,11 +4742,11 @@
       </c>
       <c r="U29" s="3">
         <f>'Laura Raw Data Pos'!F28*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P29</f>
-        <v>1.2739407496619981E-20</v>
+        <v>1.283027250830859E-20</v>
       </c>
       <c r="V29" s="3">
         <f t="shared" si="0"/>
-        <v>3.2799033939611234E-2</v>
+        <v>3.303297610710125E-2</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -4819,11 +4815,11 @@
       </c>
       <c r="U30" s="3">
         <f>'Laura Raw Data Pos'!F29*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P30</f>
-        <v>5.0724612397804597E-21</v>
+        <v>5.1753498094835685E-21</v>
       </c>
       <c r="V30" s="3">
         <f t="shared" si="0"/>
-        <v>5.8925606058105951E-3</v>
+        <v>6.0120838715313945E-3</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -4892,11 +4888,11 @@
       </c>
       <c r="U31" s="3">
         <f>'Laura Raw Data Pos'!F30*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P31</f>
-        <v>3.4723005355427597E-22</v>
+        <v>4.269355411474901E-22</v>
       </c>
       <c r="V31" s="3">
         <f t="shared" si="0"/>
-        <v>5.0140258734977469E-4</v>
+        <v>6.1649786005480865E-4</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -4965,11 +4961,11 @@
       </c>
       <c r="U32" s="3">
         <f>'Laura Raw Data Pos'!F31*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P32</f>
-        <v>4.7778681703720553E-22</v>
+        <v>9.4870137176679535E-22</v>
       </c>
       <c r="V32" s="3">
         <f t="shared" si="0"/>
-        <v>2.6682035842441257E-4</v>
+        <v>5.2980289749776969E-4</v>
       </c>
     </row>
     <row r="33" spans="1:22">
@@ -5278,11 +5274,11 @@
       </c>
       <c r="U37" s="3">
         <f>'Laura Raw Data Pos'!F36*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P37</f>
-        <v>6.4027688008478308E-22</v>
+        <v>6.0048733051848789E-20</v>
       </c>
       <c r="V37" s="3">
         <f t="shared" ref="V37:V66" si="2">U37/T37</f>
-        <v>0.42836415422032276</v>
+        <v>40.174376970086819</v>
       </c>
     </row>
     <row r="38" spans="1:22">
@@ -5351,11 +5347,11 @@
       </c>
       <c r="U38" s="3">
         <f>'Laura Raw Data Pos'!F37*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P38</f>
-        <v>2.4852582127212125E-22</v>
+        <v>3.476063109573245E-22</v>
       </c>
       <c r="V38" s="3">
         <f t="shared" si="2"/>
-        <v>3.7152374856002028E-2</v>
+        <v>5.1964016861081049E-2</v>
       </c>
     </row>
     <row r="39" spans="1:22">
@@ -5424,11 +5420,11 @@
       </c>
       <c r="U39" s="3">
         <f>'Laura Raw Data Pos'!F38*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P39</f>
-        <v>1.3531488185975821E-21</v>
+        <v>1.4483927932479319E-21</v>
       </c>
       <c r="V39" s="3">
         <f t="shared" si="2"/>
-        <v>0.21476771058212457</v>
+        <v>0.22988454777051132</v>
       </c>
     </row>
     <row r="40" spans="1:22">
@@ -5497,11 +5493,11 @@
       </c>
       <c r="U40" s="3">
         <f>'Laura Raw Data Pos'!F39*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P40</f>
-        <v>5.1072517090785123E-23</v>
+        <v>5.5226146194483665E-23</v>
       </c>
       <c r="V40" s="3">
         <f t="shared" si="2"/>
-        <v>0.66368190069233557</v>
+        <v>0.71765786693291533</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -5570,11 +5566,11 @@
       </c>
       <c r="U41" s="3">
         <f>'Laura Raw Data Pos'!F40*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P41</f>
-        <v>2.7374291447454681E-22</v>
+        <v>3.0651124486278012E-22</v>
       </c>
       <c r="V41" s="3">
         <f t="shared" si="2"/>
-        <v>3.4213370663677488E-2</v>
+        <v>3.8308874051425329E-2</v>
       </c>
     </row>
     <row r="42" spans="1:22">
@@ -5643,11 +5639,11 @@
       </c>
       <c r="U42" s="3">
         <f>'Laura Raw Data Pos'!F41*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P42</f>
-        <v>6.9748927463245703E-23</v>
+        <v>9.0732092676367526E-23</v>
       </c>
       <c r="V42" s="3">
         <f t="shared" si="2"/>
-        <v>5.9382231726646814E-3</v>
+        <v>7.7246695373069342E-3</v>
       </c>
     </row>
     <row r="43" spans="1:22">
@@ -5716,11 +5712,11 @@
       </c>
       <c r="U43" s="3">
         <f>'Laura Raw Data Pos'!F42*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P43</f>
-        <v>1.8716024093253434E-21</v>
+        <v>1.9467477850219994E-21</v>
       </c>
       <c r="V43" s="3">
         <f t="shared" si="2"/>
-        <v>0.42181610391106311</v>
+        <v>0.43875214195277651</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -5789,11 +5785,11 @@
       </c>
       <c r="U44" s="3">
         <f>'Laura Raw Data Pos'!F43*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P44</f>
-        <v>5.6160073411802892E-23</v>
+        <v>1.3607658122349514E-19</v>
       </c>
       <c r="V44" s="3">
         <f t="shared" si="2"/>
-        <v>1.7948943011808771E-3</v>
+        <v>4.3490520101581058</v>
       </c>
     </row>
     <row r="45" spans="1:22">
@@ -5862,11 +5858,11 @@
       </c>
       <c r="U45" s="3">
         <f>'Laura Raw Data Pos'!F44*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P45</f>
-        <v>2.5077057378155055E-22</v>
+        <v>2.5555937822123102E-22</v>
       </c>
       <c r="V45" s="3">
         <f t="shared" si="2"/>
-        <v>2.7577058750288742E-2</v>
+        <v>2.8103680113334917E-2</v>
       </c>
     </row>
     <row r="46" spans="1:22">
@@ -5935,11 +5931,11 @@
       </c>
       <c r="U46" s="3">
         <f>'Laura Raw Data Pos'!F45*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P46</f>
-        <v>6.0105298167542467E-23</v>
+        <v>1.5500111640196957E-22</v>
       </c>
       <c r="V46" s="3">
         <f t="shared" si="2"/>
-        <v>2.052027569793622E-4</v>
+        <v>5.2918224167032156E-4</v>
       </c>
     </row>
     <row r="47" spans="1:22">
@@ -6008,11 +6004,11 @@
       </c>
       <c r="U47" s="3">
         <f>'Laura Raw Data Pos'!F46*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P47</f>
-        <v>7.3982834728837656E-23</v>
+        <v>7.9024788224337681E-23</v>
       </c>
       <c r="V47" s="3">
         <f t="shared" si="2"/>
-        <v>2.0144077118214377E-4</v>
+        <v>2.1516902320331348E-4</v>
       </c>
     </row>
     <row r="48" spans="1:22">
@@ -6081,11 +6077,11 @@
       </c>
       <c r="U48" s="3">
         <f>'Laura Raw Data Pos'!F47*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P48</f>
-        <v>1.2043690755328615E-22</v>
+        <v>1.3199549643638246E-22</v>
       </c>
       <c r="V48" s="3">
         <f t="shared" si="2"/>
-        <v>5.3504917165930112E-3</v>
+        <v>5.8639899068977435E-3</v>
       </c>
     </row>
     <row r="49" spans="1:22">
@@ -6154,11 +6150,11 @@
       </c>
       <c r="U49" s="3">
         <f>'Laura Raw Data Pos'!F48*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P49</f>
-        <v>1.0386432079397537E-22</v>
+        <v>1.3550031630762042E-22</v>
       </c>
       <c r="V49" s="3">
         <f t="shared" si="2"/>
-        <v>6.3573056487247117E-3</v>
+        <v>8.2936750530061398E-3</v>
       </c>
     </row>
     <row r="50" spans="1:22">
@@ -6227,11 +6223,11 @@
       </c>
       <c r="U50" s="3">
         <f>'Laura Raw Data Pos'!F49*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P50</f>
-        <v>1.2180024121893962E-22</v>
+        <v>1.3073555178975188E-22</v>
       </c>
       <c r="V50" s="3">
         <f t="shared" si="2"/>
-        <v>9.7425648412630753E-3</v>
+        <v>1.0457282987481536E-2</v>
       </c>
     </row>
     <row r="51" spans="1:22">
@@ -6300,11 +6296,11 @@
       </c>
       <c r="U51" s="3">
         <f>'Laura Raw Data Pos'!F50*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P51</f>
-        <v>1.0347203822620775E-22</v>
+        <v>1.0415491863576023E-20</v>
       </c>
       <c r="V51" s="3">
         <f t="shared" si="2"/>
-        <v>4.2976036933087623E-2</v>
+        <v>4.3259664222207519</v>
       </c>
     </row>
     <row r="52" spans="1:22">
@@ -6373,11 +6369,11 @@
       </c>
       <c r="U52" s="3">
         <f>'Laura Raw Data Pos'!F51*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P52</f>
-        <v>3.0184124832857752E-23</v>
+        <v>6.5694467899994129E-22</v>
       </c>
       <c r="V52" s="3">
         <f t="shared" si="2"/>
-        <v>2.5974278867999276E-3</v>
+        <v>5.6531916653808773E-2</v>
       </c>
     </row>
     <row r="53" spans="1:22">
@@ -6446,11 +6442,11 @@
       </c>
       <c r="U53" s="3">
         <f>'Laura Raw Data Pos'!F52*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P53</f>
-        <v>6.0922339765174931E-23</v>
+        <v>7.3432311670477311E-23</v>
       </c>
       <c r="V53" s="3">
         <f t="shared" si="2"/>
-        <v>1.9774462258998575E-4</v>
+        <v>2.3835008328897602E-4</v>
       </c>
     </row>
     <row r="54" spans="1:22">
@@ -6519,11 +6515,11 @@
       </c>
       <c r="U54" s="3">
         <f>'Laura Raw Data Pos'!F53*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P54</f>
-        <v>5.3828236857872166E-23</v>
+        <v>8.3425082734181202E-23</v>
       </c>
       <c r="V54" s="3">
         <f t="shared" si="2"/>
-        <v>3.6200675096235177E-4</v>
+        <v>5.6105205951863962E-4</v>
       </c>
     </row>
     <row r="55" spans="1:22">
@@ -6592,11 +6588,11 @@
       </c>
       <c r="U55" s="3">
         <f>'Laura Raw Data Pos'!F54*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P55</f>
-        <v>3.1042587714197113E-22</v>
+        <v>3.5589123989460565E-20</v>
       </c>
       <c r="V55" s="3">
         <f t="shared" si="2"/>
-        <v>8.5133168060732081E-3</v>
+        <v>0.97601878478169302</v>
       </c>
     </row>
     <row r="56" spans="1:22">
@@ -6665,11 +6661,11 @@
       </c>
       <c r="U56" s="3">
         <f>'Laura Raw Data Pos'!F55*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P56</f>
-        <v>5.0389757786924791E-23</v>
+        <v>6.9004260769861246E-23</v>
       </c>
       <c r="V56" s="3">
         <f t="shared" si="2"/>
-        <v>2.7020786630803425E-3</v>
+        <v>3.7002547516959009E-3</v>
       </c>
     </row>
     <row r="57" spans="1:22">
@@ -6738,11 +6734,11 @@
       </c>
       <c r="U57" s="3">
         <f>'Laura Raw Data Pos'!F56*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P57</f>
-        <v>4.8700319758651603E-23</v>
+        <v>6.6308320438738977E-23</v>
       </c>
       <c r="V57" s="3">
         <f t="shared" si="2"/>
-        <v>3.7795824224670516E-5</v>
+        <v>5.1461214964414759E-5</v>
       </c>
     </row>
     <row r="58" spans="1:22">
@@ -6811,11 +6807,11 @@
       </c>
       <c r="U58" s="3">
         <f>'Laura Raw Data Pos'!F57*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P58</f>
-        <v>1.0988920355721379E-22</v>
+        <v>1.8945513198701721E-22</v>
       </c>
       <c r="V58" s="3">
         <f t="shared" si="2"/>
-        <v>3.2358963035760633E-4</v>
+        <v>5.5788661801622398E-4</v>
       </c>
     </row>
     <row r="59" spans="1:22">
@@ -6884,11 +6880,11 @@
       </c>
       <c r="U59" s="3">
         <f>'Laura Raw Data Pos'!F58*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P59</f>
-        <v>2.277361339023141E-21</v>
+        <v>2.3112224702261547E-21</v>
       </c>
       <c r="V59" s="3">
         <f t="shared" si="2"/>
-        <v>4.9051994050364775E-4</v>
+        <v>4.9781327589952008E-4</v>
       </c>
     </row>
     <row r="60" spans="1:22">
@@ -6957,11 +6953,11 @@
       </c>
       <c r="U60" s="3">
         <f>'Laura Raw Data Pos'!F59*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P60</f>
-        <v>1.0592947794937722E-22</v>
+        <v>1.3970554221490413E-22</v>
       </c>
       <c r="V60" s="3">
         <f t="shared" si="2"/>
-        <v>3.0099359134522869E-5</v>
+        <v>3.9696667722833494E-5</v>
       </c>
     </row>
     <row r="61" spans="1:22">
@@ -7030,11 +7026,11 @@
       </c>
       <c r="U61" s="3">
         <f>'Laura Raw Data Pos'!F60*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P61</f>
-        <v>4.8819290248338765E-22</v>
+        <v>3.8325558001184293E-20</v>
       </c>
       <c r="V61" s="3">
         <f t="shared" si="2"/>
-        <v>7.2680788889106286E-4</v>
+        <v>5.7058014894758952E-2</v>
       </c>
     </row>
     <row r="62" spans="1:22">
@@ -7103,11 +7099,11 @@
       </c>
       <c r="U62" s="3">
         <f>'Laura Raw Data Pos'!F61*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P62</f>
-        <v>5.9990488298555692E-21</v>
+        <v>6.0178686822672888E-21</v>
       </c>
       <c r="V62" s="3">
         <f t="shared" si="2"/>
-        <v>4.9913247742844113E-2</v>
+        <v>5.0069832558629408E-2</v>
       </c>
     </row>
     <row r="63" spans="1:22">
@@ -7176,11 +7172,11 @@
       </c>
       <c r="U63" s="3">
         <f>'Laura Raw Data Pos'!F62*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P63</f>
-        <v>2.8191291841986409E-22</v>
+        <v>3.1368798850362335E-22</v>
       </c>
       <c r="V63" s="3">
         <f t="shared" si="2"/>
-        <v>2.6614210539756475E-3</v>
+        <v>2.9613960994133307E-3</v>
       </c>
     </row>
     <row r="64" spans="1:22">
@@ -7249,11 +7245,11 @@
       </c>
       <c r="U64" s="3">
         <f>'Laura Raw Data Pos'!F63*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P64</f>
-        <v>8.6370496070958576E-23</v>
+        <v>1.1808314792308727E-20</v>
       </c>
       <c r="V64" s="3">
         <f t="shared" si="2"/>
-        <v>2.2933447497986009E-3</v>
+        <v>0.31353920568734583</v>
       </c>
     </row>
     <row r="65" spans="1:22">
@@ -7322,11 +7318,11 @@
       </c>
       <c r="U65" s="3">
         <f>'Laura Raw Data Pos'!F64*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P65</f>
-        <v>2.5267677445722529E-21</v>
+        <v>2.5528522718789471E-21</v>
       </c>
       <c r="V65" s="3">
         <f t="shared" si="2"/>
-        <v>2.8083073750669495E-2</v>
+        <v>2.8372983144074885E-2</v>
       </c>
     </row>
     <row r="66" spans="1:22">
@@ -7395,11 +7391,11 @@
       </c>
       <c r="U66" s="3">
         <f>'Laura Raw Data Pos'!F65*'Laura Raw Data Pos'!$I$2/'Data Compare'!$P66</f>
-        <v>1.700008074528444E-22</v>
+        <v>1.7555025417823971E-22</v>
       </c>
       <c r="V66" s="3">
         <f t="shared" si="2"/>
-        <v>3.4032251087835107E-2</v>
+        <v>3.5143187954470904E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8574,8 +8570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{458C70B3-3CD2-4865-9F18-7B434BF66FD8}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8631,7 +8627,7 @@
         <v>27587817064.426701</v>
       </c>
       <c r="F2" s="3">
-        <v>6706485.73169077</v>
+        <v>6939454.0509462198</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
@@ -8658,7 +8654,7 @@
         <v>13250777352.7199</v>
       </c>
       <c r="F3" s="3">
-        <v>2134255.0217172601</v>
+        <v>4005189.08937658</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
@@ -8685,7 +8681,7 @@
         <v>46808917166.408203</v>
       </c>
       <c r="F4" s="3">
-        <v>2003918.0719661801</v>
+        <v>2183900.1678089802</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>24</v>
@@ -8711,7 +8707,7 @@
         <v>15174917765.540701</v>
       </c>
       <c r="F5" s="3">
-        <v>3081751.5331749399</v>
+        <v>3356296.1765309102</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8731,7 +8727,7 @@
         <v>4139676845.4921098</v>
       </c>
       <c r="F6" s="3">
-        <v>164811260.24779001</v>
+        <v>169998653.04063401</v>
       </c>
       <c r="I6">
         <v>-3186.47229496</v>
@@ -8758,7 +8754,7 @@
         <v>71035541195.794495</v>
       </c>
       <c r="F7" s="3">
-        <v>7989090.5771990903</v>
+        <v>127663041.89713199</v>
       </c>
       <c r="I7">
         <v>-3187.33873434</v>
@@ -8785,7 +8781,7 @@
         <v>140095.67382445201</v>
       </c>
       <c r="F8" s="3">
-        <v>7607474.6113462504</v>
+        <v>98564714.377169102</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8805,7 +8801,7 @@
         <v>238250.35528425701</v>
       </c>
       <c r="F9" s="3">
-        <v>105418706.562231</v>
+        <v>106370265.42866699</v>
       </c>
       <c r="I9">
         <f>I6-I7</f>
@@ -8829,7 +8825,7 @@
         <v>64357426210.094597</v>
       </c>
       <c r="F10" s="3">
-        <v>2379863.0985081899</v>
+        <v>2444042.11851259</v>
       </c>
       <c r="I10" s="10">
         <f>I9/$I$4</f>
@@ -8853,7 +8849,7 @@
         <v>2388022987.42981</v>
       </c>
       <c r="F11" s="3">
-        <v>20458585.0880991</v>
+        <v>20709104.999638099</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -8873,7 +8869,7 @@
         <v>610900368.09290195</v>
       </c>
       <c r="F12" s="3">
-        <v>14121658.1091344</v>
+        <v>14367891.071051599</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -8893,7 +8889,7 @@
         <v>10388048124.400999</v>
       </c>
       <c r="F13" s="3">
-        <v>6737750.1954107201</v>
+        <v>11811367.6642427</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -8913,7 +8909,7 @@
         <v>76944950.581411093</v>
       </c>
       <c r="F14" s="3">
-        <v>1899181.9017467899</v>
+        <v>2042205.5726891099</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -8933,7 +8929,7 @@
         <v>10883420491.0292</v>
       </c>
       <c r="F15" s="3">
-        <v>476723.28151166101</v>
+        <v>493173.86229968199</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -8953,7 +8949,7 @@
         <v>22382338981.6819</v>
       </c>
       <c r="F16" s="3">
-        <v>592331.47358258301</v>
+        <v>2406082.2818200402</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -8973,7 +8969,7 @@
         <v>4705051412.5014296</v>
       </c>
       <c r="F17" s="3">
-        <v>33292440.817867201</v>
+        <v>33567838.417936496</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -8993,7 +8989,7 @@
         <v>143215939.22946101</v>
       </c>
       <c r="F18" s="3">
-        <v>1139224.7700404399</v>
+        <v>1477573.60819453</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -9013,7 +9009,7 @@
         <v>1319016952.39884</v>
       </c>
       <c r="F19" s="3">
-        <v>1422071.12292102</v>
+        <v>16158175.243604099</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -9033,7 +9029,7 @@
         <v>1120369539.15025</v>
       </c>
       <c r="F20" s="3">
-        <v>1022652.81836185</v>
+        <v>31404807.097201101</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -9053,7 +9049,7 @@
         <v>3857101018.47754</v>
       </c>
       <c r="F21" s="3">
-        <v>568800.89157922205</v>
+        <v>732709.67533968505</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -9073,7 +9069,7 @@
         <v>2061059507.78071</v>
       </c>
       <c r="F22" s="3">
-        <v>521026.00754259602</v>
+        <v>611541.16138872702</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -9093,7 +9089,7 @@
         <v>1520036239.0309601</v>
       </c>
       <c r="F23" s="3">
-        <v>9749840.7824942097</v>
+        <v>9818442.6273643207</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -9113,7 +9109,7 @@
         <v>6915844040.4983196</v>
       </c>
       <c r="F24" s="3">
-        <v>507823.095559109</v>
+        <v>737146.137658822</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -9133,7 +9129,7 @@
         <v>4486235650.38943</v>
       </c>
       <c r="F25" s="3">
-        <v>705276.02295508306</v>
+        <v>739225.02863745403</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -9153,7 +9149,7 @@
         <v>2287527896.9363298</v>
       </c>
       <c r="F26" s="3">
-        <v>2725528.9358988102</v>
+        <v>299169320.13724798</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -9173,7 +9169,7 @@
         <v>4434506087.0322905</v>
       </c>
       <c r="F27" s="3">
-        <v>499847.26193484798</v>
+        <v>572077.75047684601</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -9193,7 +9189,7 @@
         <v>1300091848.54705</v>
       </c>
       <c r="F28" s="3">
-        <v>42641756.665106602</v>
+        <v>42945902.970091797</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -9213,7 +9209,7 @@
         <v>2881379997.7929401</v>
       </c>
       <c r="F29" s="3">
-        <v>16978706.265365299</v>
+        <v>17323098.212484099</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -9233,7 +9229,7 @@
         <v>2318016881.59197</v>
       </c>
       <c r="F30" s="3">
-        <v>1162259.6619506699</v>
+        <v>1429052.44707237</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -9253,7 +9249,7 @@
         <v>5993783575.2308397</v>
       </c>
       <c r="F31" s="3">
-        <v>1599263.48186145</v>
+        <v>3175523.9051318401</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -9273,7 +9269,7 @@
         <v>9171584653.1112499</v>
       </c>
       <c r="F32" s="3">
-        <v>688126.22143993096</v>
+        <v>616514307.09237599</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -9293,7 +9289,7 @@
         <v>46909935.747684397</v>
       </c>
       <c r="F33" s="3">
-        <v>6042251.2098545497</v>
+        <v>6140817.9816034297</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -9313,7 +9309,7 @@
         <v>52448608.645057201</v>
       </c>
       <c r="F34" s="3">
-        <v>514072.11527513899</v>
+        <v>568759.76561518002</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -9333,7 +9329,7 @@
         <v>1822897.9971644301</v>
       </c>
       <c r="F35" s="3">
-        <v>380341.55007223599</v>
+        <v>4954019133.5933199</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -9353,7 +9349,7 @@
         <v>6637949.2019614195</v>
       </c>
       <c r="F36" s="3">
-        <v>2843459.4956556698</v>
+        <v>266675473.547885</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -9373,7 +9369,7 @@
         <v>29707367.160674401</v>
       </c>
       <c r="F37" s="3">
-        <v>1103699.2407382601</v>
+        <v>1543714.1280356101</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -9393,7 +9389,7 @@
         <v>27980521.285491198</v>
       </c>
       <c r="F38" s="3">
-        <v>6009312.4973793495</v>
+        <v>6432289.4820983103</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -9413,7 +9409,7 @@
         <v>341748.41927527997</v>
       </c>
       <c r="F39" s="3">
-        <v>226812.240463219</v>
+        <v>245258.44160479301</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -9433,7 +9429,7 @@
         <v>35543108.340276301</v>
       </c>
       <c r="F40" s="3">
-        <v>1216049.54018512</v>
+        <v>1361616.46080381</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -9453,7 +9449,7 @@
         <v>52178236.812305696</v>
       </c>
       <c r="F41" s="3">
-        <v>309846.014947619</v>
+        <v>403059.63641440502</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -9473,7 +9469,7 @@
         <v>19710553.527247898</v>
       </c>
       <c r="F42" s="3">
-        <v>8314228.8947941698</v>
+        <v>8648047.5791548695</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -9493,7 +9489,7 @@
         <v>138994357.14379099</v>
       </c>
       <c r="F43" s="3">
-        <v>249480.17953369001</v>
+        <v>604493688.33683801</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -9513,7 +9509,7 @@
         <v>40395874.1380658</v>
       </c>
       <c r="F44" s="3">
-        <v>1113999.39437471</v>
+        <v>1135272.7246747401</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -9533,7 +9529,7 @@
         <v>1301181696.8100801</v>
       </c>
       <c r="F45" s="3">
-        <v>267006.07151651301</v>
+        <v>688562.24713835097</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -9553,7 +9549,7 @@
         <v>1631518390.15712</v>
       </c>
       <c r="F46" s="3">
-        <v>328654.32271109999</v>
+        <v>351052.21834835003</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -9573,7 +9569,7 @@
         <v>99994078.086056307</v>
       </c>
       <c r="F47" s="3">
-        <v>535017.48650779901</v>
+        <v>586364.26464617904</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -9593,7 +9589,7 @@
         <v>72762546.854402095</v>
       </c>
       <c r="F48" s="3">
-        <v>462573.75013308699</v>
+        <v>603468.91963954503</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -9613,7 +9609,7 @@
         <v>55678745.561679497</v>
       </c>
       <c r="F49" s="3">
-        <v>542453.78891485103</v>
+        <v>582248.39872646402</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -9633,7 +9629,7 @@
         <v>10722874.879512601</v>
       </c>
       <c r="F50" s="3">
-        <v>460826.66685081099</v>
+        <v>46386796.678445898</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -9653,7 +9649,7 @@
         <v>51754687.184411399</v>
       </c>
       <c r="F51" s="3">
-        <v>134429.06776539699</v>
+        <v>2925791.66235309</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -9673,7 +9669,7 @@
         <v>1372102294.9096701</v>
       </c>
       <c r="F52" s="3">
-        <v>271325.85046176601</v>
+        <v>327040.69627271499</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -9693,7 +9689,7 @@
         <v>662228829.92161298</v>
       </c>
       <c r="F53" s="3">
-        <v>239731.30711352301</v>
+        <v>371544.84890013997</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -9713,7 +9709,7 @@
         <v>162395398.93691599</v>
       </c>
       <c r="F54" s="3">
-        <v>1382523.4789986101</v>
+        <v>158500959.92454699</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -9733,7 +9729,7 @@
         <v>83053680.207040399</v>
       </c>
       <c r="F55" s="3">
-        <v>224417.577177742</v>
+        <v>307319.77483193303</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -9753,7 +9749,7 @@
         <v>5738555559.7132301</v>
       </c>
       <c r="F56" s="3">
-        <v>216893.437238427</v>
+        <v>295313.04124364001</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -9773,7 +9769,7 @@
         <v>1512429112.5564001</v>
       </c>
       <c r="F57" s="3">
-        <v>489406.37747420801</v>
+        <v>843763.96259336895</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -9793,7 +9789,7 @@
         <v>20677111772.365299</v>
       </c>
       <c r="F58" s="3">
-        <v>10142535.6363679</v>
+        <v>10293340.7475417</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -9813,7 +9809,7 @@
         <v>15673795702.131201</v>
       </c>
       <c r="F59" s="3">
-        <v>471771.20583958802</v>
+        <v>622197.45994307799</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -9833,7 +9829,7 @@
         <v>4112782219.4096398</v>
       </c>
       <c r="F60" s="3">
-        <v>2989202.5623578201</v>
+        <v>234667189.133975</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -9853,7 +9849,7 @@
         <v>735919739.710307</v>
       </c>
       <c r="F61" s="3">
-        <v>36732144.287009902</v>
+        <v>36847378.143885203</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -9873,7 +9869,7 @@
         <v>648582571.07232404</v>
       </c>
       <c r="F62" s="3">
-        <v>1726151.3098935401</v>
+        <v>1920709.89612105</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -9893,7 +9889,7 @@
         <v>230314948.77973199</v>
       </c>
       <c r="F63" s="3">
-        <v>528191.57858413202</v>
+        <v>72212766.098318905</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -9913,7 +9909,7 @@
         <v>550233138.000947</v>
       </c>
       <c r="F64" s="3">
-        <v>15452237.794542899</v>
+        <v>15611755.5498123</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -9933,7 +9929,7 @@
         <v>30548252.1015983</v>
       </c>
       <c r="F65" s="3">
-        <v>1039625.7858160801</v>
+        <v>1073562.96528703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>